<commit_message>
adding hex color code to each
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AM168"/>
+  <dimension ref="A1:AN168"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -541,6 +541,11 @@
       <c r="AM1" t="n">
         <v>1984</v>
       </c>
+      <c r="AN1" t="inlineStr">
+        <is>
+          <t>Hex Color Code</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -661,6 +666,11 @@
       </c>
       <c r="AM2" t="n">
         <v>4</v>
+      </c>
+      <c r="AN2" t="inlineStr">
+        <is>
+          <t>#EE7F2D</t>
+        </is>
       </c>
     </row>
     <row r="3">
@@ -781,6 +791,11 @@
       <c r="AM3" t="n">
         <v>10</v>
       </c>
+      <c r="AN3" t="inlineStr">
+        <is>
+          <t>#8C1515</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -902,6 +917,11 @@
       <c r="AM4" t="n">
         <v>2</v>
       </c>
+      <c r="AN4" t="inlineStr">
+        <is>
+          <t>#A51C30</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -1023,6 +1043,11 @@
       <c r="AM5" t="n">
         <v>3</v>
       </c>
+      <c r="AN5" t="inlineStr">
+        <is>
+          <t>#0F4D92</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -1144,6 +1169,11 @@
       <c r="AM6" t="n">
         <v>1</v>
       </c>
+      <c r="AN6" t="inlineStr">
+        <is>
+          <t>#8C1515</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -1265,6 +1295,11 @@
       <c r="AM7" t="n">
         <v>6</v>
       </c>
+      <c r="AN7" t="inlineStr">
+        <is>
+          <t>#7A121C</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -1382,6 +1417,11 @@
       </c>
       <c r="AL8" t="inlineStr"/>
       <c r="AM8" t="inlineStr"/>
+      <c r="AN8" t="inlineStr">
+        <is>
+          <t>#990000</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1499,6 +1539,11 @@
       </c>
       <c r="AL9" t="inlineStr"/>
       <c r="AM9" t="inlineStr"/>
+      <c r="AN9" t="inlineStr">
+        <is>
+          <t>#002D72</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1618,6 +1663,11 @@
       <c r="AM10" t="n">
         <v>12</v>
       </c>
+      <c r="AN10" t="inlineStr">
+        <is>
+          <t>#F58025</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1737,6 +1787,11 @@
         <v>6</v>
       </c>
       <c r="AM11" t="inlineStr"/>
+      <c r="AN11" t="inlineStr">
+        <is>
+          <t>#001A57</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1854,6 +1909,11 @@
       </c>
       <c r="AL12" t="inlineStr"/>
       <c r="AM12" t="inlineStr"/>
+      <c r="AN12" t="inlineStr">
+        <is>
+          <t>#4E2A84</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -1975,6 +2035,11 @@
       <c r="AM13" t="n">
         <v>10</v>
       </c>
+      <c r="AN13" t="inlineStr">
+        <is>
+          <t>#00693E</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -2094,6 +2159,11 @@
         <v>7</v>
       </c>
       <c r="AM14" t="inlineStr"/>
+      <c r="AN14" t="inlineStr">
+        <is>
+          <t>#4E3629</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -2205,6 +2275,11 @@
       <c r="AK15" t="inlineStr"/>
       <c r="AL15" t="inlineStr"/>
       <c r="AM15" t="inlineStr"/>
+      <c r="AN15" t="inlineStr">
+        <is>
+          <t>#866D4B</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -2322,6 +2397,11 @@
       </c>
       <c r="AL16" t="inlineStr"/>
       <c r="AM16" t="inlineStr"/>
+      <c r="AN16" t="inlineStr">
+        <is>
+          <t>#F1C400</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -2439,6 +2519,11 @@
       </c>
       <c r="AL17" t="inlineStr"/>
       <c r="AM17" t="inlineStr"/>
+      <c r="AN17" t="inlineStr">
+        <is>
+          <t>#003D79</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -2558,6 +2643,11 @@
       <c r="AM18" t="n">
         <v>8</v>
       </c>
+      <c r="AN18" t="inlineStr">
+        <is>
+          <t>#B31B1B</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -2675,6 +2765,11 @@
       </c>
       <c r="AL19" t="inlineStr"/>
       <c r="AM19" t="inlineStr"/>
+      <c r="AN19" t="inlineStr">
+        <is>
+          <t>#9BDDFF</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -2784,6 +2879,11 @@
       <c r="AK20" t="inlineStr"/>
       <c r="AL20" t="inlineStr"/>
       <c r="AM20" t="inlineStr"/>
+      <c r="AN20" t="inlineStr">
+        <is>
+          <t>#0C2340</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -2897,6 +2997,11 @@
       <c r="AK21" t="inlineStr"/>
       <c r="AL21" t="inlineStr"/>
       <c r="AM21" t="inlineStr"/>
+      <c r="AN21" t="inlineStr">
+        <is>
+          <t>#2774AE</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -3017,6 +3122,11 @@
       </c>
       <c r="AM22" t="n">
         <v>5</v>
+      </c>
+      <c r="AN22" t="inlineStr">
+        <is>
+          <t>#003262</t>
+        </is>
       </c>
     </row>
     <row r="23">
@@ -3129,6 +3239,11 @@
       </c>
       <c r="AL23" t="inlineStr"/>
       <c r="AM23" t="inlineStr"/>
+      <c r="AN23" t="inlineStr">
+        <is>
+          <t>#002878</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -3244,6 +3359,11 @@
       <c r="AK24" t="inlineStr"/>
       <c r="AL24" t="inlineStr"/>
       <c r="AM24" t="inlineStr"/>
+      <c r="AN24" t="inlineStr">
+        <is>
+          <t>#00205B</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -3357,6 +3477,11 @@
       <c r="AM25" t="n">
         <v>13</v>
       </c>
+      <c r="AN25" t="inlineStr">
+        <is>
+          <t>#A6192E</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -3476,6 +3601,11 @@
       <c r="AM26" t="n">
         <v>7</v>
       </c>
+      <c r="AN26" t="inlineStr">
+        <is>
+          <t>#FFCB05</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -3593,6 +3723,11 @@
       </c>
       <c r="AL27" t="inlineStr"/>
       <c r="AM27" t="inlineStr"/>
+      <c r="AN27" t="inlineStr">
+        <is>
+          <t>#232D4B</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -3694,6 +3829,11 @@
       <c r="AK28" t="inlineStr"/>
       <c r="AL28" t="inlineStr"/>
       <c r="AM28" t="inlineStr"/>
+      <c r="AN28" t="inlineStr">
+        <is>
+          <t>#990000</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -3795,6 +3935,11 @@
       <c r="AK29" t="inlineStr"/>
       <c r="AL29" t="inlineStr"/>
       <c r="AM29" t="inlineStr"/>
+      <c r="AN29" t="inlineStr">
+        <is>
+          <t>#57068C</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -3884,6 +4029,11 @@
       <c r="AK30" t="inlineStr"/>
       <c r="AL30" t="inlineStr"/>
       <c r="AM30" t="inlineStr"/>
+      <c r="AN30" t="inlineStr">
+        <is>
+          <t>#FA4616</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -3997,6 +4147,11 @@
         <v>9</v>
       </c>
       <c r="AM31" t="inlineStr"/>
+      <c r="AN31" t="inlineStr">
+        <is>
+          <t>#4B9CD3</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -4098,6 +4253,11 @@
       <c r="AK32" t="inlineStr"/>
       <c r="AL32" t="inlineStr"/>
       <c r="AM32" t="inlineStr"/>
+      <c r="AN32" t="inlineStr">
+        <is>
+          <t>#9E7E38</t>
+        </is>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -4199,6 +4359,11 @@
       <c r="AK33" t="inlineStr"/>
       <c r="AL33" t="inlineStr"/>
       <c r="AM33" t="inlineStr"/>
+      <c r="AN33" t="inlineStr">
+        <is>
+          <t>#3E8EDE</t>
+        </is>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -4298,6 +4463,11 @@
       <c r="AK34" t="inlineStr"/>
       <c r="AL34" t="inlineStr"/>
       <c r="AM34" t="inlineStr"/>
+      <c r="AN34" t="inlineStr">
+        <is>
+          <t>#003C7D</t>
+        </is>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -4399,6 +4569,11 @@
       <c r="AK35" t="inlineStr"/>
       <c r="AL35" t="inlineStr"/>
       <c r="AM35" t="inlineStr"/>
+      <c r="AN35" t="inlineStr">
+        <is>
+          <t>#003B5C</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -4500,6 +4675,11 @@
       <c r="AK36" t="inlineStr"/>
       <c r="AL36" t="inlineStr"/>
       <c r="AM36" t="inlineStr"/>
+      <c r="AN36" t="inlineStr">
+        <is>
+          <t>#002244</t>
+        </is>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -4603,6 +4783,11 @@
       <c r="AK37" t="inlineStr"/>
       <c r="AL37" t="inlineStr"/>
       <c r="AM37" t="inlineStr"/>
+      <c r="AN37" t="inlineStr">
+        <is>
+          <t>#0055A2</t>
+        </is>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -4704,6 +4889,11 @@
       <c r="AK38" t="inlineStr"/>
       <c r="AL38" t="inlineStr"/>
       <c r="AM38" t="inlineStr"/>
+      <c r="AN38" t="inlineStr">
+        <is>
+          <t>#A6192E</t>
+        </is>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -4805,6 +4995,11 @@
       <c r="AK39" t="inlineStr"/>
       <c r="AL39" t="inlineStr"/>
       <c r="AM39" t="inlineStr"/>
+      <c r="AN39" t="inlineStr">
+        <is>
+          <t>#00274C</t>
+        </is>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -4900,6 +5095,11 @@
       </c>
       <c r="AL40" t="inlineStr"/>
       <c r="AM40" t="inlineStr"/>
+      <c r="AN40" t="inlineStr">
+        <is>
+          <t>#BF5700</t>
+        </is>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -5005,6 +5205,11 @@
       <c r="AM41" t="n">
         <v>13</v>
       </c>
+      <c r="AN41" t="inlineStr">
+        <is>
+          <t>#C5050C</t>
+        </is>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -5108,6 +5313,11 @@
       </c>
       <c r="AL42" t="inlineStr"/>
       <c r="AM42" t="inlineStr"/>
+      <c r="AN42" t="inlineStr">
+        <is>
+          <t>#00674E</t>
+        </is>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -5185,6 +5395,11 @@
       <c r="AK43" t="inlineStr"/>
       <c r="AL43" t="inlineStr"/>
       <c r="AM43" t="inlineStr"/>
+      <c r="AN43" t="inlineStr">
+        <is>
+          <t>#CC0000</t>
+        </is>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -5289,6 +5504,11 @@
       <c r="AL44" t="inlineStr"/>
       <c r="AM44" t="n">
         <v>8</v>
+      </c>
+      <c r="AN44" t="inlineStr">
+        <is>
+          <t>#E84A27</t>
+        </is>
       </c>
     </row>
     <row r="45">
@@ -5391,6 +5611,11 @@
       <c r="AK45" t="inlineStr"/>
       <c r="AL45" t="inlineStr"/>
       <c r="AM45" t="inlineStr"/>
+      <c r="AN45" t="inlineStr">
+        <is>
+          <t>#EEB211</t>
+        </is>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -5492,6 +5717,11 @@
       <c r="AK46" t="inlineStr"/>
       <c r="AL46" t="inlineStr"/>
       <c r="AM46" t="inlineStr"/>
+      <c r="AN46" t="inlineStr">
+        <is>
+          <t>#0038B8</t>
+        </is>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -5593,6 +5823,11 @@
       <c r="AK47" t="inlineStr"/>
       <c r="AL47" t="inlineStr"/>
       <c r="AM47" t="inlineStr"/>
+      <c r="AN47" t="inlineStr">
+        <is>
+          <t>#00294D</t>
+        </is>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -5694,6 +5929,11 @@
       <c r="AK48" t="inlineStr"/>
       <c r="AL48" t="inlineStr"/>
       <c r="AM48" t="inlineStr"/>
+      <c r="AN48" t="inlineStr">
+        <is>
+          <t>#4F8577</t>
+        </is>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -5771,6 +6011,11 @@
       <c r="AK49" t="inlineStr"/>
       <c r="AL49" t="inlineStr"/>
       <c r="AM49" t="inlineStr"/>
+      <c r="AN49" t="inlineStr">
+        <is>
+          <t>#CC0000</t>
+        </is>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -5848,6 +6093,11 @@
       <c r="AK50" t="inlineStr"/>
       <c r="AL50" t="inlineStr"/>
       <c r="AM50" t="inlineStr"/>
+      <c r="AN50" t="inlineStr">
+        <is>
+          <t>#BA0C2F</t>
+        </is>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -5923,6 +6173,11 @@
       <c r="AK51" t="inlineStr"/>
       <c r="AL51" t="inlineStr"/>
       <c r="AM51" t="inlineStr"/>
+      <c r="AN51" t="inlineStr">
+        <is>
+          <t>#BB0000</t>
+        </is>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -6024,6 +6279,11 @@
       <c r="AK52" t="inlineStr"/>
       <c r="AL52" t="inlineStr"/>
       <c r="AM52" t="inlineStr"/>
+      <c r="AN52" t="inlineStr">
+        <is>
+          <t>#B3A369</t>
+        </is>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -6099,6 +6359,11 @@
       <c r="AK53" t="inlineStr"/>
       <c r="AL53" t="inlineStr"/>
       <c r="AM53" t="inlineStr"/>
+      <c r="AN53" t="inlineStr">
+        <is>
+          <t>#CEB888</t>
+        </is>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -6158,6 +6423,11 @@
       <c r="AK54" t="inlineStr"/>
       <c r="AL54" t="inlineStr"/>
       <c r="AM54" t="inlineStr"/>
+      <c r="AN54" t="inlineStr">
+        <is>
+          <t>#001F5B</t>
+        </is>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -6253,6 +6523,11 @@
       <c r="AK55" t="inlineStr"/>
       <c r="AL55" t="inlineStr"/>
       <c r="AM55" t="inlineStr"/>
+      <c r="AN55" t="inlineStr">
+        <is>
+          <t>#AC1E2D</t>
+        </is>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -6344,6 +6619,11 @@
       <c r="AK56" t="inlineStr"/>
       <c r="AL56" t="inlineStr"/>
       <c r="AM56" t="inlineStr"/>
+      <c r="AN56" t="inlineStr">
+        <is>
+          <t>#002D72</t>
+        </is>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -6419,6 +6699,11 @@
       <c r="AK57" t="inlineStr"/>
       <c r="AL57" t="inlineStr"/>
       <c r="AM57" t="inlineStr"/>
+      <c r="AN57" t="inlineStr">
+        <is>
+          <t>#782F40</t>
+        </is>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -6468,6 +6753,11 @@
       <c r="AK58" t="inlineStr"/>
       <c r="AL58" t="inlineStr"/>
       <c r="AM58" t="inlineStr"/>
+      <c r="AN58" t="inlineStr">
+        <is>
+          <t>#8C1515</t>
+        </is>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -6545,6 +6835,11 @@
       <c r="AK59" t="inlineStr"/>
       <c r="AL59" t="inlineStr"/>
       <c r="AM59" t="inlineStr"/>
+      <c r="AN59" t="inlineStr">
+        <is>
+          <t>#005030</t>
+        </is>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -6620,6 +6915,11 @@
       <c r="AK60" t="inlineStr"/>
       <c r="AL60" t="inlineStr"/>
       <c r="AM60" t="inlineStr"/>
+      <c r="AN60" t="inlineStr">
+        <is>
+          <t>#C60C30</t>
+        </is>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -6715,6 +7015,11 @@
       <c r="AK61" t="inlineStr"/>
       <c r="AL61" t="inlineStr"/>
       <c r="AM61" t="inlineStr"/>
+      <c r="AN61" t="inlineStr">
+        <is>
+          <t>#4B2E83</t>
+        </is>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -6800,6 +7105,11 @@
       <c r="AK62" t="inlineStr"/>
       <c r="AL62" t="inlineStr"/>
       <c r="AM62" t="inlineStr"/>
+      <c r="AN62" t="inlineStr">
+        <is>
+          <t>#CC0033</t>
+        </is>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -6891,6 +7201,11 @@
       <c r="AK63" t="inlineStr"/>
       <c r="AL63" t="inlineStr"/>
       <c r="AM63" t="inlineStr"/>
+      <c r="AN63" t="inlineStr">
+        <is>
+          <t>#D44500</t>
+        </is>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -6966,6 +7281,11 @@
       <c r="AK64" t="inlineStr"/>
       <c r="AL64" t="inlineStr"/>
       <c r="AM64" t="inlineStr"/>
+      <c r="AN64" t="inlineStr">
+        <is>
+          <t>#003594</t>
+        </is>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -7053,6 +7373,11 @@
       <c r="AK65" t="inlineStr"/>
       <c r="AL65" t="inlineStr"/>
       <c r="AM65" t="inlineStr"/>
+      <c r="AN65" t="inlineStr">
+        <is>
+          <t>#002244</t>
+        </is>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -7128,6 +7453,11 @@
       <c r="AK66" t="inlineStr"/>
       <c r="AL66" t="inlineStr"/>
       <c r="AM66" t="inlineStr"/>
+      <c r="AN66" t="inlineStr">
+        <is>
+          <t>#7A0019</t>
+        </is>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -7203,6 +7533,11 @@
       <c r="AK67" t="inlineStr"/>
       <c r="AL67" t="inlineStr"/>
       <c r="AM67" t="inlineStr"/>
+      <c r="AN67" t="inlineStr">
+        <is>
+          <t>#660000</t>
+        </is>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -7268,6 +7603,11 @@
       <c r="AK68" t="inlineStr"/>
       <c r="AL68" t="inlineStr"/>
       <c r="AM68" t="inlineStr"/>
+      <c r="AN68" t="inlineStr">
+        <is>
+          <t>#001E62</t>
+        </is>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -7353,6 +7693,11 @@
       <c r="AK69" t="inlineStr"/>
       <c r="AL69" t="inlineStr"/>
       <c r="AM69" t="inlineStr"/>
+      <c r="AN69" t="inlineStr">
+        <is>
+          <t>#C21E56</t>
+        </is>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -7440,6 +7785,11 @@
       <c r="AK70" t="inlineStr"/>
       <c r="AL70" t="inlineStr"/>
       <c r="AM70" t="inlineStr"/>
+      <c r="AN70" t="inlineStr">
+        <is>
+          <t>#500000</t>
+        </is>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -7515,6 +7865,11 @@
       <c r="AK71" t="inlineStr"/>
       <c r="AL71" t="inlineStr"/>
       <c r="AM71" t="inlineStr"/>
+      <c r="AN71" t="inlineStr">
+        <is>
+          <t>#880029</t>
+        </is>
+      </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -7612,6 +7967,11 @@
       <c r="AK72" t="inlineStr"/>
       <c r="AL72" t="inlineStr"/>
       <c r="AM72" t="inlineStr"/>
+      <c r="AN72" t="inlineStr">
+        <is>
+          <t>#003399</t>
+        </is>
+      </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -7687,6 +8047,11 @@
       <c r="AK73" t="inlineStr"/>
       <c r="AL73" t="inlineStr"/>
       <c r="AM73" t="inlineStr"/>
+      <c r="AN73" t="inlineStr">
+        <is>
+          <t>#8C2633</t>
+        </is>
+      </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
@@ -7762,6 +8127,11 @@
       <c r="AK74" t="inlineStr"/>
       <c r="AL74" t="inlineStr"/>
       <c r="AM74" t="inlineStr"/>
+      <c r="AN74" t="inlineStr">
+        <is>
+          <t>#990000</t>
+        </is>
+      </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
@@ -7837,6 +8207,11 @@
       <c r="AK75" t="inlineStr"/>
       <c r="AL75" t="inlineStr"/>
       <c r="AM75" t="inlineStr"/>
+      <c r="AN75" t="inlineStr">
+        <is>
+          <t>#C41230</t>
+        </is>
+      </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -7912,6 +8287,11 @@
       <c r="AK76" t="inlineStr"/>
       <c r="AL76" t="inlineStr"/>
       <c r="AM76" t="inlineStr"/>
+      <c r="AN76" t="inlineStr">
+        <is>
+          <t>#9B2743</t>
+        </is>
+      </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
@@ -7987,6 +8367,11 @@
       <c r="AK77" t="inlineStr"/>
       <c r="AL77" t="inlineStr"/>
       <c r="AM77" t="inlineStr"/>
+      <c r="AN77" t="inlineStr">
+        <is>
+          <t>#CC0000</t>
+        </is>
+      </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
@@ -8084,6 +8469,11 @@
       <c r="AK78" t="inlineStr"/>
       <c r="AL78" t="inlineStr"/>
       <c r="AM78" t="inlineStr"/>
+      <c r="AN78" t="inlineStr">
+        <is>
+          <t>#002D62</t>
+        </is>
+      </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
@@ -8159,6 +8549,11 @@
       <c r="AK79" t="inlineStr"/>
       <c r="AL79" t="inlineStr"/>
       <c r="AM79" t="inlineStr"/>
+      <c r="AN79" t="inlineStr">
+        <is>
+          <t>#003015</t>
+        </is>
+      </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
@@ -8234,6 +8629,11 @@
       <c r="AK80" t="inlineStr"/>
       <c r="AL80" t="inlineStr"/>
       <c r="AM80" t="inlineStr"/>
+      <c r="AN80" t="inlineStr">
+        <is>
+          <t>#F66733</t>
+        </is>
+      </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
@@ -8283,6 +8683,11 @@
       <c r="AK81" t="inlineStr"/>
       <c r="AL81" t="inlineStr"/>
       <c r="AM81" t="inlineStr"/>
+      <c r="AN81" t="inlineStr">
+        <is>
+          <t>#98002E</t>
+        </is>
+      </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
@@ -8358,6 +8763,11 @@
       <c r="AK82" t="inlineStr"/>
       <c r="AL82" t="inlineStr"/>
       <c r="AM82" t="inlineStr"/>
+      <c r="AN82" t="inlineStr">
+        <is>
+          <t>#18453B</t>
+        </is>
+      </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
@@ -8433,6 +8843,11 @@
       <c r="AK83" t="inlineStr"/>
       <c r="AL83" t="inlineStr"/>
       <c r="AM83" t="inlineStr"/>
+      <c r="AN83" t="inlineStr">
+        <is>
+          <t>#E03A3E</t>
+        </is>
+      </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
@@ -8482,6 +8897,11 @@
       <c r="AK84" t="inlineStr"/>
       <c r="AL84" t="inlineStr"/>
       <c r="AM84" t="inlineStr"/>
+      <c r="AN84" t="inlineStr">
+        <is>
+          <t>#041E42</t>
+        </is>
+      </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
@@ -8557,6 +8977,11 @@
       <c r="AK85" t="inlineStr"/>
       <c r="AL85" t="inlineStr"/>
       <c r="AM85" t="inlineStr"/>
+      <c r="AN85" t="inlineStr">
+        <is>
+          <t>#006C5C</t>
+        </is>
+      </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
@@ -8632,6 +9057,11 @@
       <c r="AK86" t="inlineStr"/>
       <c r="AL86" t="inlineStr"/>
       <c r="AM86" t="inlineStr"/>
+      <c r="AN86" t="inlineStr">
+        <is>
+          <t>#00386B</t>
+        </is>
+      </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
@@ -8707,6 +9137,11 @@
       <c r="AK87" t="inlineStr"/>
       <c r="AL87" t="inlineStr"/>
       <c r="AM87" t="inlineStr"/>
+      <c r="AN87" t="inlineStr">
+        <is>
+          <t>#E2231A</t>
+        </is>
+      </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
@@ -8782,6 +9217,11 @@
       <c r="AK88" t="inlineStr"/>
       <c r="AL88" t="inlineStr"/>
       <c r="AM88" t="inlineStr"/>
+      <c r="AN88" t="inlineStr">
+        <is>
+          <t>#000000</t>
+        </is>
+      </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
@@ -8857,6 +9297,11 @@
       <c r="AK89" t="inlineStr"/>
       <c r="AL89" t="inlineStr"/>
       <c r="AM89" t="inlineStr"/>
+      <c r="AN89" t="inlineStr">
+        <is>
+          <t>#003B5C</t>
+        </is>
+      </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
@@ -8932,6 +9377,11 @@
       <c r="AK90" t="inlineStr"/>
       <c r="AL90" t="inlineStr"/>
       <c r="AM90" t="inlineStr"/>
+      <c r="AN90" t="inlineStr">
+        <is>
+          <t>#002E5D</t>
+        </is>
+      </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
@@ -9007,6 +9457,11 @@
       <c r="AK91" t="inlineStr"/>
       <c r="AL91" t="inlineStr"/>
       <c r="AM91" t="inlineStr"/>
+      <c r="AN91" t="inlineStr">
+        <is>
+          <t>#E87722</t>
+        </is>
+      </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
@@ -9056,6 +9511,11 @@
       <c r="AK92" t="inlineStr"/>
       <c r="AL92" t="inlineStr"/>
       <c r="AM92" t="inlineStr"/>
+      <c r="AN92" t="inlineStr">
+        <is>
+          <t>#7E3E89</t>
+        </is>
+      </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
@@ -9131,6 +9591,11 @@
       <c r="AK93" t="inlineStr"/>
       <c r="AL93" t="inlineStr"/>
       <c r="AM93" t="inlineStr"/>
+      <c r="AN93" t="inlineStr">
+        <is>
+          <t>#2A2554</t>
+        </is>
+      </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
@@ -9206,6 +9671,11 @@
       <c r="AK94" t="inlineStr"/>
       <c r="AL94" t="inlineStr"/>
       <c r="AM94" t="inlineStr"/>
+      <c r="AN94" t="inlineStr">
+        <is>
+          <t>#4D1979</t>
+        </is>
+      </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
@@ -9281,6 +9751,11 @@
       <c r="AK95" t="inlineStr"/>
       <c r="AL95" t="inlineStr"/>
       <c r="AM95" t="inlineStr"/>
+      <c r="AN95" t="inlineStr">
+        <is>
+          <t>#005482</t>
+        </is>
+      </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
@@ -9356,6 +9831,11 @@
       <c r="AK96" t="inlineStr"/>
       <c r="AL96" t="inlineStr"/>
       <c r="AM96" t="inlineStr"/>
+      <c r="AN96" t="inlineStr">
+        <is>
+          <t>#005BBB</t>
+        </is>
+      </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
@@ -9431,6 +9911,11 @@
       <c r="AK97" t="inlineStr"/>
       <c r="AL97" t="inlineStr"/>
       <c r="AM97" t="inlineStr"/>
+      <c r="AN97" t="inlineStr">
+        <is>
+          <t>#00539B</t>
+        </is>
+      </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
@@ -9480,6 +9965,11 @@
       <c r="AK98" t="inlineStr"/>
       <c r="AL98" t="inlineStr"/>
       <c r="AM98" t="inlineStr"/>
+      <c r="AN98" t="inlineStr">
+        <is>
+          <t>#003366</t>
+        </is>
+      </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
@@ -9555,6 +10045,11 @@
       <c r="AK99" t="inlineStr"/>
       <c r="AL99" t="inlineStr"/>
       <c r="AM99" t="inlineStr"/>
+      <c r="AN99" t="inlineStr">
+        <is>
+          <t>#002654</t>
+        </is>
+      </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
@@ -9630,6 +10125,11 @@
       <c r="AK100" t="inlineStr"/>
       <c r="AL100" t="inlineStr"/>
       <c r="AM100" t="inlineStr"/>
+      <c r="AN100" t="inlineStr">
+        <is>
+          <t>#0C2340</t>
+        </is>
+      </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
@@ -9705,6 +10205,11 @@
       <c r="AK101" t="inlineStr"/>
       <c r="AL101" t="inlineStr"/>
       <c r="AM101" t="inlineStr"/>
+      <c r="AN101" t="inlineStr">
+        <is>
+          <t>#C1B998</t>
+        </is>
+      </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
@@ -9780,6 +10285,11 @@
       <c r="AK102" t="inlineStr"/>
       <c r="AL102" t="inlineStr"/>
       <c r="AM102" t="inlineStr"/>
+      <c r="AN102" t="inlineStr">
+        <is>
+          <t>#EE2E24</t>
+        </is>
+      </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
@@ -9829,6 +10339,11 @@
       <c r="AK103" t="inlineStr"/>
       <c r="AL103" t="inlineStr"/>
       <c r="AM103" t="inlineStr"/>
+      <c r="AN103" t="inlineStr">
+        <is>
+          <t>#C8102E</t>
+        </is>
+      </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
@@ -9878,6 +10393,11 @@
       <c r="AK104" t="inlineStr"/>
       <c r="AL104" t="inlineStr"/>
       <c r="AM104" t="inlineStr"/>
+      <c r="AN104" t="inlineStr">
+        <is>
+          <t>#003E7E</t>
+        </is>
+      </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
@@ -9927,6 +10447,11 @@
       <c r="AK105" t="inlineStr"/>
       <c r="AL105" t="inlineStr"/>
       <c r="AM105" t="inlineStr"/>
+      <c r="AN105" t="inlineStr">
+        <is>
+          <t>#006747</t>
+        </is>
+      </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
@@ -10002,6 +10527,11 @@
       <c r="AK106" t="inlineStr"/>
       <c r="AL106" t="inlineStr"/>
       <c r="AM106" t="inlineStr"/>
+      <c r="AN106" t="inlineStr">
+        <is>
+          <t>#C8102E</t>
+        </is>
+      </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
@@ -10077,6 +10607,11 @@
       <c r="AK107" t="inlineStr"/>
       <c r="AL107" t="inlineStr"/>
       <c r="AM107" t="inlineStr"/>
+      <c r="AN107" t="inlineStr">
+        <is>
+          <t>#154733</t>
+        </is>
+      </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
@@ -10126,6 +10661,11 @@
       <c r="AK108" t="inlineStr"/>
       <c r="AL108" t="inlineStr"/>
       <c r="AM108" t="inlineStr"/>
+      <c r="AN108" t="inlineStr">
+        <is>
+          <t>#CC0000</t>
+        </is>
+      </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
@@ -10201,6 +10741,11 @@
       <c r="AK109" t="inlineStr"/>
       <c r="AL109" t="inlineStr"/>
       <c r="AM109" t="inlineStr"/>
+      <c r="AN109" t="inlineStr">
+        <is>
+          <t>#E0A458</t>
+        </is>
+      </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
@@ -10276,6 +10821,11 @@
       <c r="AK110" t="inlineStr"/>
       <c r="AL110" t="inlineStr"/>
       <c r="AM110" t="inlineStr"/>
+      <c r="AN110" t="inlineStr">
+        <is>
+          <t>#AB0D3B</t>
+        </is>
+      </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
@@ -10351,6 +10901,11 @@
       <c r="AK111" t="inlineStr"/>
       <c r="AL111" t="inlineStr"/>
       <c r="AM111" t="inlineStr"/>
+      <c r="AN111" t="inlineStr">
+        <is>
+          <t>#003DA5</t>
+        </is>
+      </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
@@ -10426,6 +10981,11 @@
       <c r="AK112" t="inlineStr"/>
       <c r="AL112" t="inlineStr"/>
       <c r="AM112" t="inlineStr"/>
+      <c r="AN112" t="inlineStr">
+        <is>
+          <t>#CC0033</t>
+        </is>
+      </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
@@ -10475,6 +11035,11 @@
       <c r="AK113" t="inlineStr"/>
       <c r="AL113" t="inlineStr"/>
       <c r="AM113" t="inlineStr"/>
+      <c r="AN113" t="inlineStr">
+        <is>
+          <t>#007A33</t>
+        </is>
+      </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
@@ -10524,6 +11089,11 @@
       <c r="AK114" t="inlineStr"/>
       <c r="AL114" t="inlineStr"/>
       <c r="AM114" t="inlineStr"/>
+      <c r="AN114" t="inlineStr">
+        <is>
+          <t>#F36E21</t>
+        </is>
+      </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
@@ -10573,6 +11143,11 @@
       <c r="AK115" t="inlineStr"/>
       <c r="AL115" t="inlineStr"/>
       <c r="AM115" t="inlineStr"/>
+      <c r="AN115" t="inlineStr">
+        <is>
+          <t>#00594C</t>
+        </is>
+      </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
@@ -10622,6 +11197,11 @@
       <c r="AK116" t="inlineStr"/>
       <c r="AL116" t="inlineStr"/>
       <c r="AM116" t="inlineStr"/>
+      <c r="AN116" t="inlineStr">
+        <is>
+          <t>#0051BA</t>
+        </is>
+      </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
@@ -10697,6 +11277,11 @@
       <c r="AK117" t="inlineStr"/>
       <c r="AL117" t="inlineStr"/>
       <c r="AM117" t="inlineStr"/>
+      <c r="AN117" t="inlineStr">
+        <is>
+          <t>#CC0000</t>
+        </is>
+      </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
@@ -10772,6 +11357,11 @@
       <c r="AK118" t="inlineStr"/>
       <c r="AL118" t="inlineStr"/>
       <c r="AM118" t="inlineStr"/>
+      <c r="AN118" t="inlineStr">
+        <is>
+          <t>#FF8200</t>
+        </is>
+      </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
@@ -10847,6 +11437,11 @@
       <c r="AK119" t="inlineStr"/>
       <c r="AL119" t="inlineStr"/>
       <c r="AM119" t="inlineStr"/>
+      <c r="AN119" t="inlineStr">
+        <is>
+          <t>#73000A</t>
+        </is>
+      </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
@@ -10896,6 +11491,11 @@
       <c r="AK120" t="inlineStr"/>
       <c r="AL120" t="inlineStr"/>
       <c r="AM120" t="inlineStr"/>
+      <c r="AN120" t="inlineStr">
+        <is>
+          <t>#CC0033</t>
+        </is>
+      </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
@@ -10943,6 +11543,11 @@
       <c r="AK121" t="inlineStr"/>
       <c r="AL121" t="inlineStr"/>
       <c r="AM121" t="inlineStr"/>
+      <c r="AN121" t="inlineStr">
+        <is>
+          <t>#C8102E</t>
+        </is>
+      </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
@@ -10992,6 +11597,11 @@
       <c r="AK122" t="inlineStr"/>
       <c r="AL122" t="inlineStr"/>
       <c r="AM122" t="inlineStr"/>
+      <c r="AN122" t="inlineStr">
+        <is>
+          <t>#A41E35</t>
+        </is>
+      </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
@@ -11067,6 +11677,11 @@
       <c r="AK123" t="inlineStr"/>
       <c r="AL123" t="inlineStr"/>
       <c r="AM123" t="inlineStr"/>
+      <c r="AN123" t="inlineStr">
+        <is>
+          <t>#8C1D40</t>
+        </is>
+      </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
@@ -11116,6 +11731,11 @@
       <c r="AK124" t="inlineStr"/>
       <c r="AL124" t="inlineStr"/>
       <c r="AM124" t="inlineStr"/>
+      <c r="AN124" t="inlineStr">
+        <is>
+          <t>#E35205</t>
+        </is>
+      </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
@@ -11191,6 +11811,11 @@
       <c r="AK125" t="inlineStr"/>
       <c r="AL125" t="inlineStr"/>
       <c r="AM125" t="inlineStr"/>
+      <c r="AN125" t="inlineStr">
+        <is>
+          <t>#00563F</t>
+        </is>
+      </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
@@ -11266,6 +11891,11 @@
       <c r="AK126" t="inlineStr"/>
       <c r="AL126" t="inlineStr"/>
       <c r="AM126" t="inlineStr"/>
+      <c r="AN126" t="inlineStr">
+        <is>
+          <t>#0051BA</t>
+        </is>
+      </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
@@ -11341,6 +11971,11 @@
       <c r="AK127" t="inlineStr"/>
       <c r="AL127" t="inlineStr"/>
       <c r="AM127" t="inlineStr"/>
+      <c r="AN127" t="inlineStr">
+        <is>
+          <t>#F1B82D</t>
+        </is>
+      </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
@@ -11416,6 +12051,11 @@
       <c r="AK128" t="inlineStr"/>
       <c r="AL128" t="inlineStr"/>
       <c r="AM128" t="inlineStr"/>
+      <c r="AN128" t="inlineStr">
+        <is>
+          <t>#B5072D</t>
+        </is>
+      </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
@@ -11491,6 +12131,11 @@
       <c r="AK129" t="inlineStr"/>
       <c r="AL129" t="inlineStr"/>
       <c r="AM129" t="inlineStr"/>
+      <c r="AN129" t="inlineStr">
+        <is>
+          <t>#C8102E</t>
+        </is>
+      </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
@@ -11566,6 +12211,11 @@
       <c r="AK130" t="inlineStr"/>
       <c r="AL130" t="inlineStr"/>
       <c r="AM130" t="inlineStr"/>
+      <c r="AN130" t="inlineStr">
+        <is>
+          <t>#9D2235</t>
+        </is>
+      </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
@@ -11615,6 +12265,11 @@
       <c r="AK131" t="inlineStr"/>
       <c r="AL131" t="inlineStr"/>
       <c r="AM131" t="inlineStr"/>
+      <c r="AN131" t="inlineStr">
+        <is>
+          <t>#CBA93E</t>
+        </is>
+      </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
@@ -11690,6 +12345,11 @@
       <c r="AK132" t="inlineStr"/>
       <c r="AL132" t="inlineStr"/>
       <c r="AM132" t="inlineStr"/>
+      <c r="AN132" t="inlineStr">
+        <is>
+          <t>#CE1141</t>
+        </is>
+      </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
@@ -11765,6 +12425,11 @@
       <c r="AK133" t="inlineStr"/>
       <c r="AL133" t="inlineStr"/>
       <c r="AM133" t="inlineStr"/>
+      <c r="AN133" t="inlineStr">
+        <is>
+          <t>#841617</t>
+        </is>
+      </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
@@ -11814,6 +12479,11 @@
       <c r="AK134" t="inlineStr"/>
       <c r="AL134" t="inlineStr"/>
       <c r="AM134" t="inlineStr"/>
+      <c r="AN134" t="inlineStr">
+        <is>
+          <t>#E82E21</t>
+        </is>
+      </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
@@ -11863,6 +12533,11 @@
       <c r="AK135" t="inlineStr"/>
       <c r="AL135" t="inlineStr"/>
       <c r="AM135" t="inlineStr"/>
+      <c r="AN135" t="inlineStr">
+        <is>
+          <t>#8A2432</t>
+        </is>
+      </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
@@ -11912,6 +12587,11 @@
       <c r="AK136" t="inlineStr"/>
       <c r="AL136" t="inlineStr"/>
       <c r="AM136" t="inlineStr"/>
+      <c r="AN136" t="inlineStr">
+        <is>
+          <t>#CC0033</t>
+        </is>
+      </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
@@ -11961,6 +12641,11 @@
       <c r="AK137" t="inlineStr"/>
       <c r="AL137" t="inlineStr"/>
       <c r="AM137" t="inlineStr"/>
+      <c r="AN137" t="inlineStr">
+        <is>
+          <t>#1A2650</t>
+        </is>
+      </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
@@ -12010,6 +12695,11 @@
       <c r="AK138" t="inlineStr"/>
       <c r="AL138" t="inlineStr"/>
       <c r="AM138" t="inlineStr"/>
+      <c r="AN138" t="inlineStr">
+        <is>
+          <t>#004489</t>
+        </is>
+      </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
@@ -12059,6 +12749,11 @@
       <c r="AK139" t="inlineStr"/>
       <c r="AL139" t="inlineStr"/>
       <c r="AM139" t="inlineStr"/>
+      <c r="AN139" t="inlineStr">
+        <is>
+          <t>#990000</t>
+        </is>
+      </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
@@ -12108,6 +12803,11 @@
       <c r="AK140" t="inlineStr"/>
       <c r="AL140" t="inlineStr"/>
       <c r="AM140" t="inlineStr"/>
+      <c r="AN140" t="inlineStr">
+        <is>
+          <t>#004488</t>
+        </is>
+      </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
@@ -12183,6 +12883,11 @@
       <c r="AK141" t="inlineStr"/>
       <c r="AL141" t="inlineStr"/>
       <c r="AM141" t="inlineStr"/>
+      <c r="AN141" t="inlineStr">
+        <is>
+          <t>#0033A0</t>
+        </is>
+      </c>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
@@ -12232,6 +12937,11 @@
       <c r="AK142" t="inlineStr"/>
       <c r="AL142" t="inlineStr"/>
       <c r="AM142" t="inlineStr"/>
+      <c r="AN142" t="inlineStr">
+        <is>
+          <t>#004477</t>
+        </is>
+      </c>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
@@ -12307,6 +13017,11 @@
       <c r="AK143" t="inlineStr"/>
       <c r="AL143" t="inlineStr"/>
       <c r="AM143" t="inlineStr"/>
+      <c r="AN143" t="inlineStr">
+        <is>
+          <t>#005581</t>
+        </is>
+      </c>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
@@ -12356,6 +13071,11 @@
       <c r="AK144" t="inlineStr"/>
       <c r="AL144" t="inlineStr"/>
       <c r="AM144" t="inlineStr"/>
+      <c r="AN144" t="inlineStr">
+        <is>
+          <t>#512773</t>
+        </is>
+      </c>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
@@ -12431,6 +13151,11 @@
       <c r="AK145" t="inlineStr"/>
       <c r="AL145" t="inlineStr"/>
       <c r="AM145" t="inlineStr"/>
+      <c r="AN145" t="inlineStr">
+        <is>
+          <t>#CFB87C</t>
+        </is>
+      </c>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
@@ -12480,6 +13205,11 @@
       <c r="AK146" t="inlineStr"/>
       <c r="AL146" t="inlineStr"/>
       <c r="AM146" t="inlineStr"/>
+      <c r="AN146" t="inlineStr">
+        <is>
+          <t>#FFCC29</t>
+        </is>
+      </c>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
@@ -12555,6 +13285,11 @@
       <c r="AK147" t="inlineStr"/>
       <c r="AL147" t="inlineStr"/>
       <c r="AM147" t="inlineStr"/>
+      <c r="AN147" t="inlineStr">
+        <is>
+          <t>#A60C31</t>
+        </is>
+      </c>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
@@ -12604,6 +13339,11 @@
       <c r="AK148" t="inlineStr"/>
       <c r="AL148" t="inlineStr"/>
       <c r="AM148" t="inlineStr"/>
+      <c r="AN148" t="inlineStr">
+        <is>
+          <t>#006341</t>
+        </is>
+      </c>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
@@ -12653,6 +13393,11 @@
       <c r="AK149" t="inlineStr"/>
       <c r="AL149" t="inlineStr"/>
       <c r="AM149" t="inlineStr"/>
+      <c r="AN149" t="inlineStr">
+        <is>
+          <t>#FFC904</t>
+        </is>
+      </c>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
@@ -12700,6 +13445,11 @@
       <c r="AK150" t="inlineStr"/>
       <c r="AL150" t="inlineStr"/>
       <c r="AM150" t="inlineStr"/>
+      <c r="AN150" t="inlineStr">
+        <is>
+          <t>#FDBB30</t>
+        </is>
+      </c>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
@@ -12747,6 +13497,11 @@
       <c r="AK151" t="inlineStr"/>
       <c r="AL151" t="inlineStr"/>
       <c r="AM151" t="inlineStr"/>
+      <c r="AN151" t="inlineStr">
+        <is>
+          <t>#FFC72C</t>
+        </is>
+      </c>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
@@ -12820,6 +13575,11 @@
       <c r="AK152" t="inlineStr"/>
       <c r="AL152" t="inlineStr"/>
       <c r="AM152" t="inlineStr"/>
+      <c r="AN152" t="inlineStr">
+        <is>
+          <t>#990000</t>
+        </is>
+      </c>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
@@ -12867,6 +13627,11 @@
       <c r="AK153" t="inlineStr"/>
       <c r="AL153" t="inlineStr"/>
       <c r="AM153" t="inlineStr"/>
+      <c r="AN153" t="inlineStr">
+        <is>
+          <t>#006BA6</t>
+        </is>
+      </c>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr">
@@ -12914,6 +13679,11 @@
       <c r="AK154" t="inlineStr"/>
       <c r="AL154" t="inlineStr"/>
       <c r="AM154" t="inlineStr"/>
+      <c r="AN154" t="inlineStr">
+        <is>
+          <t>#FDB913</t>
+        </is>
+      </c>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
@@ -12987,6 +13757,11 @@
       <c r="AK155" t="inlineStr"/>
       <c r="AL155" t="inlineStr"/>
       <c r="AM155" t="inlineStr"/>
+      <c r="AN155" t="inlineStr">
+        <is>
+          <t>#E41C38</t>
+        </is>
+      </c>
     </row>
     <row r="156">
       <c r="A156" t="inlineStr">
@@ -13034,6 +13809,11 @@
       <c r="AK156" t="inlineStr"/>
       <c r="AL156" t="inlineStr"/>
       <c r="AM156" t="inlineStr"/>
+      <c r="AN156" t="inlineStr">
+        <is>
+          <t>#008542</t>
+        </is>
+      </c>
     </row>
     <row r="157">
       <c r="A157" t="inlineStr">
@@ -13107,6 +13887,11 @@
       <c r="AK157" t="inlineStr"/>
       <c r="AL157" t="inlineStr"/>
       <c r="AM157" t="inlineStr"/>
+      <c r="AN157" t="inlineStr">
+        <is>
+          <t>#FF6200</t>
+        </is>
+      </c>
     </row>
     <row r="158">
       <c r="A158" t="inlineStr">
@@ -13180,6 +13965,11 @@
       <c r="AK158" t="inlineStr"/>
       <c r="AL158" t="inlineStr"/>
       <c r="AM158" t="inlineStr"/>
+      <c r="AN158" t="inlineStr">
+        <is>
+          <t>#1E4D2B</t>
+        </is>
+      </c>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
@@ -13227,6 +14017,11 @@
       <c r="AK159" t="inlineStr"/>
       <c r="AL159" t="inlineStr"/>
       <c r="AM159" t="inlineStr"/>
+      <c r="AN159" t="inlineStr">
+        <is>
+          <t>#9D2235</t>
+        </is>
+      </c>
     </row>
     <row r="160">
       <c r="A160" t="inlineStr">
@@ -13274,6 +14069,11 @@
       <c r="AK160" t="inlineStr"/>
       <c r="AL160" t="inlineStr"/>
       <c r="AM160" t="inlineStr"/>
+      <c r="AN160" t="inlineStr">
+        <is>
+          <t>#00214D</t>
+        </is>
+      </c>
     </row>
     <row r="161">
       <c r="A161" t="inlineStr">
@@ -13347,6 +14147,11 @@
       <c r="AK161" t="inlineStr"/>
       <c r="AL161" t="inlineStr"/>
       <c r="AM161" t="inlineStr"/>
+      <c r="AN161" t="inlineStr">
+        <is>
+          <t>#0065A3</t>
+        </is>
+      </c>
     </row>
     <row r="162">
       <c r="A162" t="inlineStr">
@@ -13394,6 +14199,11 @@
       <c r="AK162" t="inlineStr"/>
       <c r="AL162" t="inlineStr"/>
       <c r="AM162" t="inlineStr"/>
+      <c r="AN162" t="inlineStr">
+        <is>
+          <t>#0C2340</t>
+        </is>
+      </c>
     </row>
     <row r="163">
       <c r="A163" t="inlineStr">
@@ -13441,6 +14251,11 @@
       <c r="AK163" t="inlineStr"/>
       <c r="AL163" t="inlineStr"/>
       <c r="AM163" t="inlineStr"/>
+      <c r="AN163" t="inlineStr">
+        <is>
+          <t>#C41230</t>
+        </is>
+      </c>
     </row>
     <row r="164">
       <c r="A164" t="inlineStr">
@@ -13488,6 +14303,11 @@
       <c r="AK164" t="inlineStr"/>
       <c r="AL164" t="inlineStr"/>
       <c r="AM164" t="inlineStr"/>
+      <c r="AN164" t="inlineStr">
+        <is>
+          <t>#E00122</t>
+        </is>
+      </c>
     </row>
     <row r="165">
       <c r="A165" t="inlineStr">
@@ -13535,6 +14355,11 @@
       <c r="AK165" t="inlineStr"/>
       <c r="AL165" t="inlineStr"/>
       <c r="AM165" t="inlineStr"/>
+      <c r="AN165" t="inlineStr">
+        <is>
+          <t>#CE1141</t>
+        </is>
+      </c>
     </row>
     <row r="166">
       <c r="A166" t="inlineStr">
@@ -13596,6 +14421,11 @@
       <c r="AK166" t="inlineStr"/>
       <c r="AL166" t="inlineStr"/>
       <c r="AM166" t="inlineStr"/>
+      <c r="AN166" t="inlineStr">
+        <is>
+          <t>#006A4D</t>
+        </is>
+      </c>
     </row>
     <row r="167">
       <c r="A167" t="inlineStr">
@@ -13667,6 +14497,11 @@
       <c r="AK167" t="inlineStr"/>
       <c r="AL167" t="inlineStr"/>
       <c r="AM167" t="inlineStr"/>
+      <c r="AN167" t="inlineStr">
+        <is>
+          <t>#9D2235</t>
+        </is>
+      </c>
     </row>
     <row r="168">
       <c r="A168" t="inlineStr">
@@ -13728,6 +14563,11 @@
       <c r="AK168" t="inlineStr"/>
       <c r="AL168" t="inlineStr"/>
       <c r="AM168" t="inlineStr"/>
+      <c r="AN168" t="inlineStr">
+        <is>
+          <t>#981E32</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
correcting "Instittute" typo to "Institute"
another typo...  it was a result from an error in the data I used to verify my own data
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -652,7 +652,7 @@
     <t>#007A33</t>
   </si>
   <si>
-    <t>Rochester Instittue of Technology</t>
+    <t>Rochester Institute of Technology</t>
   </si>
   <si>
     <t>#F36E21</t>
@@ -948,13 +948,19 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -990,7 +996,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
@@ -998,10 +1004,7 @@
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -1321,46 +1324,46 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="15" max="15" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="16" max="16" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="17" max="17" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="18" max="18" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="19" max="19" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="20" max="20" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="21" max="21" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="22" max="22" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="23" max="23" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="24" max="24" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="25" max="25" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="26" max="26" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="27" max="27" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="28" max="28" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="29" max="29" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="30" max="30" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="31" max="31" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="32" max="32" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="33" max="33" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="34" max="34" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="35" max="35" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="36" max="36" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="37" max="37" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="38" max="38" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="39" max="39" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="40" max="40" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="15" max="15" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="16" max="16" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="17" max="17" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="18" max="18" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="19" max="19" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="20" max="20" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="21" max="21" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="22" max="22" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="23" max="23" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="24" max="24" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="25" max="25" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="26" max="26" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="27" max="27" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="28" max="28" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="29" max="29" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="30" max="30" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="31" max="31" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="32" max="32" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="33" max="33" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="34" max="34" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="35" max="35" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="36" max="36" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="37" max="37" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="38" max="38" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="39" max="39" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="40" max="40" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
@@ -6917,7 +6920,7 @@
         <v>97</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="19.5">
       <c r="A52" s="1" t="s">
         <v>98</v>
       </c>
@@ -7019,7 +7022,7 @@
         <v>99</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="19.5">
       <c r="A53" s="1" t="s">
         <v>100</v>
       </c>
@@ -7095,7 +7098,7 @@
         <v>101</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="19.5">
       <c r="A54" s="1" t="s">
         <v>102</v>
       </c>
@@ -7121,14 +7124,14 @@
       <c r="I54" s="2">
         <v>50</v>
       </c>
-      <c r="J54" s="4"/>
-      <c r="K54" s="4"/>
-      <c r="L54" s="4"/>
-      <c r="M54" s="4"/>
-      <c r="N54" s="4"/>
-      <c r="O54" s="4"/>
-      <c r="P54" s="4"/>
-      <c r="Q54" s="4"/>
+      <c r="J54" s="3"/>
+      <c r="K54" s="3"/>
+      <c r="L54" s="3"/>
+      <c r="M54" s="3"/>
+      <c r="N54" s="3"/>
+      <c r="O54" s="3"/>
+      <c r="P54" s="3"/>
+      <c r="Q54" s="3"/>
       <c r="R54" s="3"/>
       <c r="S54" s="3"/>
       <c r="T54" s="3"/>
@@ -7155,7 +7158,7 @@
         <v>103</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="19.5">
       <c r="A55" s="1" t="s">
         <v>104</v>
       </c>
@@ -7251,7 +7254,7 @@
         <v>105</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="19.5">
       <c r="A56" s="1" t="s">
         <v>106</v>
       </c>
@@ -7343,7 +7346,7 @@
         <v>16</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="19.5">
       <c r="A57" s="1" t="s">
         <v>107</v>
       </c>
@@ -7419,7 +7422,7 @@
         <v>108</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="19.5">
       <c r="A58" s="1" t="s">
         <v>109</v>
       </c>
@@ -7435,14 +7438,14 @@
       <c r="G58" s="3"/>
       <c r="H58" s="3"/>
       <c r="I58" s="3"/>
-      <c r="J58" s="4"/>
-      <c r="K58" s="4"/>
-      <c r="L58" s="4"/>
-      <c r="M58" s="4"/>
-      <c r="N58" s="4"/>
-      <c r="O58" s="4"/>
-      <c r="P58" s="4"/>
-      <c r="Q58" s="4"/>
+      <c r="J58" s="3"/>
+      <c r="K58" s="3"/>
+      <c r="L58" s="3"/>
+      <c r="M58" s="3"/>
+      <c r="N58" s="3"/>
+      <c r="O58" s="3"/>
+      <c r="P58" s="3"/>
+      <c r="Q58" s="3"/>
       <c r="R58" s="3"/>
       <c r="S58" s="3"/>
       <c r="T58" s="3"/>
@@ -7469,7 +7472,7 @@
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="19.5">
       <c r="A59" s="1" t="s">
         <v>110</v>
       </c>
@@ -7547,7 +7550,7 @@
         <v>111</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="19.5">
       <c r="A60" s="1" t="s">
         <v>112</v>
       </c>
@@ -7623,7 +7626,7 @@
         <v>113</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="19.5">
       <c r="A61" s="1" t="s">
         <v>114</v>
       </c>
@@ -9273,14 +9276,14 @@
       <c r="G81" s="3"/>
       <c r="H81" s="3"/>
       <c r="I81" s="3"/>
-      <c r="J81" s="4"/>
-      <c r="K81" s="4"/>
-      <c r="L81" s="4"/>
-      <c r="M81" s="4"/>
-      <c r="N81" s="4"/>
-      <c r="O81" s="4"/>
-      <c r="P81" s="4"/>
-      <c r="Q81" s="4"/>
+      <c r="J81" s="3"/>
+      <c r="K81" s="3"/>
+      <c r="L81" s="3"/>
+      <c r="M81" s="3"/>
+      <c r="N81" s="3"/>
+      <c r="O81" s="3"/>
+      <c r="P81" s="3"/>
+      <c r="Q81" s="3"/>
       <c r="R81" s="3"/>
       <c r="S81" s="3"/>
       <c r="T81" s="3"/>
@@ -9475,14 +9478,14 @@
       <c r="G84" s="3"/>
       <c r="H84" s="3"/>
       <c r="I84" s="3"/>
-      <c r="J84" s="4"/>
-      <c r="K84" s="4"/>
-      <c r="L84" s="4"/>
-      <c r="M84" s="4"/>
-      <c r="N84" s="4"/>
-      <c r="O84" s="4"/>
-      <c r="P84" s="4"/>
-      <c r="Q84" s="4"/>
+      <c r="J84" s="3"/>
+      <c r="K84" s="3"/>
+      <c r="L84" s="3"/>
+      <c r="M84" s="3"/>
+      <c r="N84" s="3"/>
+      <c r="O84" s="3"/>
+      <c r="P84" s="3"/>
+      <c r="Q84" s="3"/>
       <c r="R84" s="3"/>
       <c r="S84" s="3"/>
       <c r="T84" s="3"/>
@@ -10057,14 +10060,14 @@
       <c r="G92" s="3"/>
       <c r="H92" s="3"/>
       <c r="I92" s="3"/>
-      <c r="J92" s="4"/>
-      <c r="K92" s="4"/>
-      <c r="L92" s="4"/>
-      <c r="M92" s="4"/>
-      <c r="N92" s="4"/>
-      <c r="O92" s="4"/>
-      <c r="P92" s="4"/>
-      <c r="Q92" s="4"/>
+      <c r="J92" s="3"/>
+      <c r="K92" s="3"/>
+      <c r="L92" s="3"/>
+      <c r="M92" s="3"/>
+      <c r="N92" s="3"/>
+      <c r="O92" s="3"/>
+      <c r="P92" s="3"/>
+      <c r="Q92" s="3"/>
       <c r="R92" s="3"/>
       <c r="S92" s="3"/>
       <c r="T92" s="3"/>
@@ -10487,14 +10490,14 @@
       <c r="G98" s="3"/>
       <c r="H98" s="3"/>
       <c r="I98" s="3"/>
-      <c r="J98" s="4"/>
-      <c r="K98" s="4"/>
-      <c r="L98" s="4"/>
-      <c r="M98" s="4"/>
-      <c r="N98" s="4"/>
-      <c r="O98" s="4"/>
-      <c r="P98" s="4"/>
-      <c r="Q98" s="4"/>
+      <c r="J98" s="3"/>
+      <c r="K98" s="3"/>
+      <c r="L98" s="3"/>
+      <c r="M98" s="3"/>
+      <c r="N98" s="3"/>
+      <c r="O98" s="3"/>
+      <c r="P98" s="3"/>
+      <c r="Q98" s="3"/>
       <c r="R98" s="3"/>
       <c r="S98" s="3"/>
       <c r="T98" s="3"/>
@@ -10841,14 +10844,14 @@
       <c r="G103" s="3"/>
       <c r="H103" s="3"/>
       <c r="I103" s="3"/>
-      <c r="J103" s="4"/>
-      <c r="K103" s="4"/>
-      <c r="L103" s="4"/>
-      <c r="M103" s="4"/>
-      <c r="N103" s="4"/>
-      <c r="O103" s="4"/>
-      <c r="P103" s="4"/>
-      <c r="Q103" s="4"/>
+      <c r="J103" s="3"/>
+      <c r="K103" s="3"/>
+      <c r="L103" s="3"/>
+      <c r="M103" s="3"/>
+      <c r="N103" s="3"/>
+      <c r="O103" s="3"/>
+      <c r="P103" s="3"/>
+      <c r="Q103" s="3"/>
       <c r="R103" s="3"/>
       <c r="S103" s="3"/>
       <c r="T103" s="3"/>
@@ -10891,14 +10894,14 @@
       <c r="G104" s="3"/>
       <c r="H104" s="3"/>
       <c r="I104" s="3"/>
-      <c r="J104" s="4"/>
-      <c r="K104" s="4"/>
-      <c r="L104" s="4"/>
-      <c r="M104" s="4"/>
-      <c r="N104" s="4"/>
-      <c r="O104" s="4"/>
-      <c r="P104" s="4"/>
-      <c r="Q104" s="4"/>
+      <c r="J104" s="3"/>
+      <c r="K104" s="3"/>
+      <c r="L104" s="3"/>
+      <c r="M104" s="3"/>
+      <c r="N104" s="3"/>
+      <c r="O104" s="3"/>
+      <c r="P104" s="3"/>
+      <c r="Q104" s="3"/>
       <c r="R104" s="3"/>
       <c r="S104" s="3"/>
       <c r="T104" s="3"/>
@@ -10941,14 +10944,14 @@
       <c r="G105" s="3"/>
       <c r="H105" s="3"/>
       <c r="I105" s="3"/>
-      <c r="J105" s="4"/>
-      <c r="K105" s="4"/>
-      <c r="L105" s="4"/>
-      <c r="M105" s="4"/>
-      <c r="N105" s="4"/>
-      <c r="O105" s="4"/>
-      <c r="P105" s="4"/>
-      <c r="Q105" s="4"/>
+      <c r="J105" s="3"/>
+      <c r="K105" s="3"/>
+      <c r="L105" s="3"/>
+      <c r="M105" s="3"/>
+      <c r="N105" s="3"/>
+      <c r="O105" s="3"/>
+      <c r="P105" s="3"/>
+      <c r="Q105" s="3"/>
       <c r="R105" s="3"/>
       <c r="S105" s="3"/>
       <c r="T105" s="3"/>
@@ -11143,14 +11146,14 @@
       <c r="G108" s="3"/>
       <c r="H108" s="3"/>
       <c r="I108" s="3"/>
-      <c r="J108" s="4"/>
-      <c r="K108" s="4"/>
-      <c r="L108" s="4"/>
-      <c r="M108" s="4"/>
-      <c r="N108" s="4"/>
-      <c r="O108" s="4"/>
-      <c r="P108" s="4"/>
-      <c r="Q108" s="4"/>
+      <c r="J108" s="3"/>
+      <c r="K108" s="3"/>
+      <c r="L108" s="3"/>
+      <c r="M108" s="3"/>
+      <c r="N108" s="3"/>
+      <c r="O108" s="3"/>
+      <c r="P108" s="3"/>
+      <c r="Q108" s="3"/>
       <c r="R108" s="3"/>
       <c r="S108" s="3"/>
       <c r="T108" s="3"/>
@@ -11497,14 +11500,14 @@
       <c r="G113" s="3"/>
       <c r="H113" s="3"/>
       <c r="I113" s="3"/>
-      <c r="J113" s="4"/>
-      <c r="K113" s="4"/>
-      <c r="L113" s="4"/>
-      <c r="M113" s="4"/>
-      <c r="N113" s="4"/>
-      <c r="O113" s="4"/>
-      <c r="P113" s="4"/>
-      <c r="Q113" s="4"/>
+      <c r="J113" s="3"/>
+      <c r="K113" s="3"/>
+      <c r="L113" s="3"/>
+      <c r="M113" s="3"/>
+      <c r="N113" s="3"/>
+      <c r="O113" s="3"/>
+      <c r="P113" s="3"/>
+      <c r="Q113" s="3"/>
       <c r="R113" s="3"/>
       <c r="S113" s="3"/>
       <c r="T113" s="3"/>
@@ -11547,14 +11550,14 @@
       <c r="G114" s="3"/>
       <c r="H114" s="3"/>
       <c r="I114" s="3"/>
-      <c r="J114" s="4"/>
-      <c r="K114" s="4"/>
-      <c r="L114" s="4"/>
-      <c r="M114" s="4"/>
-      <c r="N114" s="4"/>
-      <c r="O114" s="4"/>
-      <c r="P114" s="4"/>
-      <c r="Q114" s="4"/>
+      <c r="J114" s="3"/>
+      <c r="K114" s="3"/>
+      <c r="L114" s="3"/>
+      <c r="M114" s="3"/>
+      <c r="N114" s="3"/>
+      <c r="O114" s="3"/>
+      <c r="P114" s="3"/>
+      <c r="Q114" s="3"/>
       <c r="R114" s="3"/>
       <c r="S114" s="3"/>
       <c r="T114" s="3"/>
@@ -11597,14 +11600,14 @@
       <c r="G115" s="3"/>
       <c r="H115" s="3"/>
       <c r="I115" s="3"/>
-      <c r="J115" s="4"/>
-      <c r="K115" s="4"/>
-      <c r="L115" s="4"/>
-      <c r="M115" s="4"/>
-      <c r="N115" s="4"/>
-      <c r="O115" s="4"/>
-      <c r="P115" s="4"/>
-      <c r="Q115" s="4"/>
+      <c r="J115" s="3"/>
+      <c r="K115" s="3"/>
+      <c r="L115" s="3"/>
+      <c r="M115" s="3"/>
+      <c r="N115" s="3"/>
+      <c r="O115" s="3"/>
+      <c r="P115" s="3"/>
+      <c r="Q115" s="3"/>
       <c r="R115" s="3"/>
       <c r="S115" s="3"/>
       <c r="T115" s="3"/>
@@ -11647,14 +11650,14 @@
       <c r="G116" s="3"/>
       <c r="H116" s="3"/>
       <c r="I116" s="3"/>
-      <c r="J116" s="4"/>
-      <c r="K116" s="4"/>
-      <c r="L116" s="4"/>
-      <c r="M116" s="4"/>
-      <c r="N116" s="4"/>
-      <c r="O116" s="4"/>
-      <c r="P116" s="4"/>
-      <c r="Q116" s="4"/>
+      <c r="J116" s="3"/>
+      <c r="K116" s="3"/>
+      <c r="L116" s="3"/>
+      <c r="M116" s="3"/>
+      <c r="N116" s="3"/>
+      <c r="O116" s="3"/>
+      <c r="P116" s="3"/>
+      <c r="Q116" s="3"/>
       <c r="R116" s="3"/>
       <c r="S116" s="3"/>
       <c r="T116" s="3"/>
@@ -11925,14 +11928,14 @@
       <c r="G120" s="3"/>
       <c r="H120" s="3"/>
       <c r="I120" s="3"/>
-      <c r="J120" s="4"/>
-      <c r="K120" s="4"/>
-      <c r="L120" s="4"/>
-      <c r="M120" s="4"/>
-      <c r="N120" s="4"/>
-      <c r="O120" s="4"/>
-      <c r="P120" s="4"/>
-      <c r="Q120" s="4"/>
+      <c r="J120" s="3"/>
+      <c r="K120" s="3"/>
+      <c r="L120" s="3"/>
+      <c r="M120" s="3"/>
+      <c r="N120" s="3"/>
+      <c r="O120" s="3"/>
+      <c r="P120" s="3"/>
+      <c r="Q120" s="3"/>
       <c r="R120" s="3"/>
       <c r="S120" s="3"/>
       <c r="T120" s="3"/>
@@ -11973,14 +11976,14 @@
       <c r="G121" s="3"/>
       <c r="H121" s="3"/>
       <c r="I121" s="3"/>
-      <c r="J121" s="4"/>
-      <c r="K121" s="4"/>
-      <c r="L121" s="4"/>
-      <c r="M121" s="4"/>
-      <c r="N121" s="4"/>
-      <c r="O121" s="4"/>
-      <c r="P121" s="4"/>
-      <c r="Q121" s="4"/>
+      <c r="J121" s="3"/>
+      <c r="K121" s="3"/>
+      <c r="L121" s="3"/>
+      <c r="M121" s="3"/>
+      <c r="N121" s="3"/>
+      <c r="O121" s="3"/>
+      <c r="P121" s="3"/>
+      <c r="Q121" s="3"/>
       <c r="R121" s="3"/>
       <c r="S121" s="3"/>
       <c r="T121" s="3"/>
@@ -12023,14 +12026,14 @@
       <c r="G122" s="3"/>
       <c r="H122" s="3"/>
       <c r="I122" s="3"/>
-      <c r="J122" s="4"/>
-      <c r="K122" s="4"/>
-      <c r="L122" s="4"/>
-      <c r="M122" s="4"/>
-      <c r="N122" s="4"/>
-      <c r="O122" s="4"/>
-      <c r="P122" s="4"/>
-      <c r="Q122" s="4"/>
+      <c r="J122" s="3"/>
+      <c r="K122" s="3"/>
+      <c r="L122" s="3"/>
+      <c r="M122" s="3"/>
+      <c r="N122" s="3"/>
+      <c r="O122" s="3"/>
+      <c r="P122" s="3"/>
+      <c r="Q122" s="3"/>
       <c r="R122" s="3"/>
       <c r="S122" s="3"/>
       <c r="T122" s="3"/>
@@ -12149,14 +12152,14 @@
       <c r="G124" s="3"/>
       <c r="H124" s="3"/>
       <c r="I124" s="3"/>
-      <c r="J124" s="4"/>
-      <c r="K124" s="4"/>
-      <c r="L124" s="4"/>
-      <c r="M124" s="4"/>
-      <c r="N124" s="4"/>
-      <c r="O124" s="4"/>
-      <c r="P124" s="4"/>
-      <c r="Q124" s="4"/>
+      <c r="J124" s="3"/>
+      <c r="K124" s="3"/>
+      <c r="L124" s="3"/>
+      <c r="M124" s="3"/>
+      <c r="N124" s="3"/>
+      <c r="O124" s="3"/>
+      <c r="P124" s="3"/>
+      <c r="Q124" s="3"/>
       <c r="R124" s="3"/>
       <c r="S124" s="3"/>
       <c r="T124" s="3"/>
@@ -12655,14 +12658,14 @@
       <c r="G131" s="3"/>
       <c r="H131" s="3"/>
       <c r="I131" s="3"/>
-      <c r="J131" s="4"/>
-      <c r="K131" s="4"/>
-      <c r="L131" s="4"/>
-      <c r="M131" s="4"/>
-      <c r="N131" s="4"/>
-      <c r="O131" s="4"/>
-      <c r="P131" s="4"/>
-      <c r="Q131" s="4"/>
+      <c r="J131" s="3"/>
+      <c r="K131" s="3"/>
+      <c r="L131" s="3"/>
+      <c r="M131" s="3"/>
+      <c r="N131" s="3"/>
+      <c r="O131" s="3"/>
+      <c r="P131" s="3"/>
+      <c r="Q131" s="3"/>
       <c r="R131" s="3"/>
       <c r="S131" s="3"/>
       <c r="T131" s="3"/>
@@ -12857,14 +12860,14 @@
       <c r="G134" s="3"/>
       <c r="H134" s="3"/>
       <c r="I134" s="3"/>
-      <c r="J134" s="4"/>
-      <c r="K134" s="4"/>
-      <c r="L134" s="4"/>
-      <c r="M134" s="4"/>
-      <c r="N134" s="4"/>
-      <c r="O134" s="4"/>
-      <c r="P134" s="4"/>
-      <c r="Q134" s="4"/>
+      <c r="J134" s="3"/>
+      <c r="K134" s="3"/>
+      <c r="L134" s="3"/>
+      <c r="M134" s="3"/>
+      <c r="N134" s="3"/>
+      <c r="O134" s="3"/>
+      <c r="P134" s="3"/>
+      <c r="Q134" s="3"/>
       <c r="R134" s="3"/>
       <c r="S134" s="3"/>
       <c r="T134" s="3"/>
@@ -12907,14 +12910,14 @@
       <c r="G135" s="3"/>
       <c r="H135" s="3"/>
       <c r="I135" s="3"/>
-      <c r="J135" s="4"/>
-      <c r="K135" s="4"/>
-      <c r="L135" s="4"/>
-      <c r="M135" s="4"/>
-      <c r="N135" s="4"/>
-      <c r="O135" s="4"/>
-      <c r="P135" s="4"/>
-      <c r="Q135" s="4"/>
+      <c r="J135" s="3"/>
+      <c r="K135" s="3"/>
+      <c r="L135" s="3"/>
+      <c r="M135" s="3"/>
+      <c r="N135" s="3"/>
+      <c r="O135" s="3"/>
+      <c r="P135" s="3"/>
+      <c r="Q135" s="3"/>
       <c r="R135" s="3"/>
       <c r="S135" s="3"/>
       <c r="T135" s="3"/>
@@ -12957,14 +12960,14 @@
       <c r="G136" s="3"/>
       <c r="H136" s="3"/>
       <c r="I136" s="3"/>
-      <c r="J136" s="4"/>
-      <c r="K136" s="4"/>
-      <c r="L136" s="4"/>
-      <c r="M136" s="4"/>
-      <c r="N136" s="4"/>
-      <c r="O136" s="4"/>
-      <c r="P136" s="4"/>
-      <c r="Q136" s="4"/>
+      <c r="J136" s="3"/>
+      <c r="K136" s="3"/>
+      <c r="L136" s="3"/>
+      <c r="M136" s="3"/>
+      <c r="N136" s="3"/>
+      <c r="O136" s="3"/>
+      <c r="P136" s="3"/>
+      <c r="Q136" s="3"/>
       <c r="R136" s="3"/>
       <c r="S136" s="3"/>
       <c r="T136" s="3"/>
@@ -13007,14 +13010,14 @@
       <c r="G137" s="3"/>
       <c r="H137" s="3"/>
       <c r="I137" s="3"/>
-      <c r="J137" s="4"/>
-      <c r="K137" s="4"/>
-      <c r="L137" s="4"/>
-      <c r="M137" s="4"/>
-      <c r="N137" s="4"/>
-      <c r="O137" s="4"/>
-      <c r="P137" s="4"/>
-      <c r="Q137" s="4"/>
+      <c r="J137" s="3"/>
+      <c r="K137" s="3"/>
+      <c r="L137" s="3"/>
+      <c r="M137" s="3"/>
+      <c r="N137" s="3"/>
+      <c r="O137" s="3"/>
+      <c r="P137" s="3"/>
+      <c r="Q137" s="3"/>
       <c r="R137" s="3"/>
       <c r="S137" s="3"/>
       <c r="T137" s="3"/>
@@ -13057,14 +13060,14 @@
       <c r="G138" s="3"/>
       <c r="H138" s="3"/>
       <c r="I138" s="3"/>
-      <c r="J138" s="4"/>
-      <c r="K138" s="4"/>
-      <c r="L138" s="4"/>
-      <c r="M138" s="4"/>
-      <c r="N138" s="4"/>
-      <c r="O138" s="4"/>
-      <c r="P138" s="4"/>
-      <c r="Q138" s="4"/>
+      <c r="J138" s="3"/>
+      <c r="K138" s="3"/>
+      <c r="L138" s="3"/>
+      <c r="M138" s="3"/>
+      <c r="N138" s="3"/>
+      <c r="O138" s="3"/>
+      <c r="P138" s="3"/>
+      <c r="Q138" s="3"/>
       <c r="R138" s="3"/>
       <c r="S138" s="3"/>
       <c r="T138" s="3"/>
@@ -13107,14 +13110,14 @@
       <c r="G139" s="3"/>
       <c r="H139" s="3"/>
       <c r="I139" s="3"/>
-      <c r="J139" s="4"/>
-      <c r="K139" s="4"/>
-      <c r="L139" s="4"/>
-      <c r="M139" s="4"/>
-      <c r="N139" s="4"/>
-      <c r="O139" s="4"/>
-      <c r="P139" s="4"/>
-      <c r="Q139" s="4"/>
+      <c r="J139" s="3"/>
+      <c r="K139" s="3"/>
+      <c r="L139" s="3"/>
+      <c r="M139" s="3"/>
+      <c r="N139" s="3"/>
+      <c r="O139" s="3"/>
+      <c r="P139" s="3"/>
+      <c r="Q139" s="3"/>
       <c r="R139" s="3"/>
       <c r="S139" s="3"/>
       <c r="T139" s="3"/>
@@ -13157,14 +13160,14 @@
       <c r="G140" s="3"/>
       <c r="H140" s="3"/>
       <c r="I140" s="3"/>
-      <c r="J140" s="4"/>
-      <c r="K140" s="4"/>
-      <c r="L140" s="4"/>
-      <c r="M140" s="4"/>
-      <c r="N140" s="4"/>
-      <c r="O140" s="4"/>
-      <c r="P140" s="4"/>
-      <c r="Q140" s="4"/>
+      <c r="J140" s="3"/>
+      <c r="K140" s="3"/>
+      <c r="L140" s="3"/>
+      <c r="M140" s="3"/>
+      <c r="N140" s="3"/>
+      <c r="O140" s="3"/>
+      <c r="P140" s="3"/>
+      <c r="Q140" s="3"/>
       <c r="R140" s="3"/>
       <c r="S140" s="3"/>
       <c r="T140" s="3"/>
@@ -13283,14 +13286,14 @@
       <c r="G142" s="3"/>
       <c r="H142" s="3"/>
       <c r="I142" s="3"/>
-      <c r="J142" s="4"/>
-      <c r="K142" s="4"/>
-      <c r="L142" s="4"/>
-      <c r="M142" s="4"/>
-      <c r="N142" s="4"/>
-      <c r="O142" s="4"/>
-      <c r="P142" s="4"/>
-      <c r="Q142" s="4"/>
+      <c r="J142" s="3"/>
+      <c r="K142" s="3"/>
+      <c r="L142" s="3"/>
+      <c r="M142" s="3"/>
+      <c r="N142" s="3"/>
+      <c r="O142" s="3"/>
+      <c r="P142" s="3"/>
+      <c r="Q142" s="3"/>
       <c r="R142" s="3"/>
       <c r="S142" s="3"/>
       <c r="T142" s="3"/>
@@ -13409,14 +13412,14 @@
       <c r="G144" s="3"/>
       <c r="H144" s="3"/>
       <c r="I144" s="3"/>
-      <c r="J144" s="4"/>
-      <c r="K144" s="4"/>
-      <c r="L144" s="4"/>
-      <c r="M144" s="4"/>
-      <c r="N144" s="4"/>
-      <c r="O144" s="4"/>
-      <c r="P144" s="4"/>
-      <c r="Q144" s="4"/>
+      <c r="J144" s="3"/>
+      <c r="K144" s="3"/>
+      <c r="L144" s="3"/>
+      <c r="M144" s="3"/>
+      <c r="N144" s="3"/>
+      <c r="O144" s="3"/>
+      <c r="P144" s="3"/>
+      <c r="Q144" s="3"/>
       <c r="R144" s="3"/>
       <c r="S144" s="3"/>
       <c r="T144" s="3"/>
@@ -13535,14 +13538,14 @@
       <c r="G146" s="3"/>
       <c r="H146" s="3"/>
       <c r="I146" s="3"/>
-      <c r="J146" s="4"/>
-      <c r="K146" s="4"/>
-      <c r="L146" s="4"/>
-      <c r="M146" s="4"/>
-      <c r="N146" s="4"/>
-      <c r="O146" s="4"/>
-      <c r="P146" s="4"/>
-      <c r="Q146" s="4"/>
+      <c r="J146" s="3"/>
+      <c r="K146" s="3"/>
+      <c r="L146" s="3"/>
+      <c r="M146" s="3"/>
+      <c r="N146" s="3"/>
+      <c r="O146" s="3"/>
+      <c r="P146" s="3"/>
+      <c r="Q146" s="3"/>
       <c r="R146" s="3"/>
       <c r="S146" s="3"/>
       <c r="T146" s="3"/>
@@ -13661,14 +13664,14 @@
       <c r="G148" s="3"/>
       <c r="H148" s="3"/>
       <c r="I148" s="3"/>
-      <c r="J148" s="4"/>
-      <c r="K148" s="4"/>
-      <c r="L148" s="4"/>
-      <c r="M148" s="4"/>
-      <c r="N148" s="4"/>
-      <c r="O148" s="4"/>
-      <c r="P148" s="4"/>
-      <c r="Q148" s="4"/>
+      <c r="J148" s="3"/>
+      <c r="K148" s="3"/>
+      <c r="L148" s="3"/>
+      <c r="M148" s="3"/>
+      <c r="N148" s="3"/>
+      <c r="O148" s="3"/>
+      <c r="P148" s="3"/>
+      <c r="Q148" s="3"/>
       <c r="R148" s="3"/>
       <c r="S148" s="3"/>
       <c r="T148" s="3"/>
@@ -13711,14 +13714,14 @@
       <c r="G149" s="3"/>
       <c r="H149" s="3"/>
       <c r="I149" s="3"/>
-      <c r="J149" s="4"/>
-      <c r="K149" s="4"/>
-      <c r="L149" s="4"/>
-      <c r="M149" s="4"/>
-      <c r="N149" s="4"/>
-      <c r="O149" s="4"/>
-      <c r="P149" s="4"/>
-      <c r="Q149" s="4"/>
+      <c r="J149" s="3"/>
+      <c r="K149" s="3"/>
+      <c r="L149" s="3"/>
+      <c r="M149" s="3"/>
+      <c r="N149" s="3"/>
+      <c r="O149" s="3"/>
+      <c r="P149" s="3"/>
+      <c r="Q149" s="3"/>
       <c r="R149" s="3"/>
       <c r="S149" s="3"/>
       <c r="T149" s="3"/>
@@ -13759,14 +13762,14 @@
       <c r="G150" s="3"/>
       <c r="H150" s="3"/>
       <c r="I150" s="3"/>
-      <c r="J150" s="4"/>
-      <c r="K150" s="4"/>
-      <c r="L150" s="4"/>
-      <c r="M150" s="4"/>
-      <c r="N150" s="4"/>
-      <c r="O150" s="4"/>
-      <c r="P150" s="4"/>
-      <c r="Q150" s="4"/>
+      <c r="J150" s="3"/>
+      <c r="K150" s="3"/>
+      <c r="L150" s="3"/>
+      <c r="M150" s="3"/>
+      <c r="N150" s="3"/>
+      <c r="O150" s="3"/>
+      <c r="P150" s="3"/>
+      <c r="Q150" s="3"/>
       <c r="R150" s="3"/>
       <c r="S150" s="3"/>
       <c r="T150" s="3"/>
@@ -13807,14 +13810,14 @@
       <c r="G151" s="3"/>
       <c r="H151" s="3"/>
       <c r="I151" s="3"/>
-      <c r="J151" s="4"/>
-      <c r="K151" s="4"/>
-      <c r="L151" s="4"/>
-      <c r="M151" s="4"/>
-      <c r="N151" s="4"/>
-      <c r="O151" s="4"/>
-      <c r="P151" s="4"/>
-      <c r="Q151" s="4"/>
+      <c r="J151" s="3"/>
+      <c r="K151" s="3"/>
+      <c r="L151" s="3"/>
+      <c r="M151" s="3"/>
+      <c r="N151" s="3"/>
+      <c r="O151" s="3"/>
+      <c r="P151" s="3"/>
+      <c r="Q151" s="3"/>
       <c r="R151" s="3"/>
       <c r="S151" s="3"/>
       <c r="T151" s="3"/>
@@ -13929,14 +13932,14 @@
       <c r="G153" s="3"/>
       <c r="H153" s="3"/>
       <c r="I153" s="3"/>
-      <c r="J153" s="4"/>
-      <c r="K153" s="4"/>
-      <c r="L153" s="4"/>
-      <c r="M153" s="4"/>
-      <c r="N153" s="4"/>
-      <c r="O153" s="4"/>
-      <c r="P153" s="4"/>
-      <c r="Q153" s="4"/>
+      <c r="J153" s="3"/>
+      <c r="K153" s="3"/>
+      <c r="L153" s="3"/>
+      <c r="M153" s="3"/>
+      <c r="N153" s="3"/>
+      <c r="O153" s="3"/>
+      <c r="P153" s="3"/>
+      <c r="Q153" s="3"/>
       <c r="R153" s="3"/>
       <c r="S153" s="3"/>
       <c r="T153" s="3"/>
@@ -13977,14 +13980,14 @@
       <c r="G154" s="3"/>
       <c r="H154" s="3"/>
       <c r="I154" s="3"/>
-      <c r="J154" s="4"/>
-      <c r="K154" s="4"/>
-      <c r="L154" s="4"/>
-      <c r="M154" s="4"/>
-      <c r="N154" s="4"/>
-      <c r="O154" s="4"/>
-      <c r="P154" s="4"/>
-      <c r="Q154" s="4"/>
+      <c r="J154" s="3"/>
+      <c r="K154" s="3"/>
+      <c r="L154" s="3"/>
+      <c r="M154" s="3"/>
+      <c r="N154" s="3"/>
+      <c r="O154" s="3"/>
+      <c r="P154" s="3"/>
+      <c r="Q154" s="3"/>
       <c r="R154" s="3"/>
       <c r="S154" s="3"/>
       <c r="T154" s="3"/>
@@ -14099,14 +14102,14 @@
       <c r="G156" s="3"/>
       <c r="H156" s="3"/>
       <c r="I156" s="3"/>
-      <c r="J156" s="4"/>
-      <c r="K156" s="4"/>
-      <c r="L156" s="4"/>
-      <c r="M156" s="4"/>
-      <c r="N156" s="4"/>
-      <c r="O156" s="4"/>
-      <c r="P156" s="4"/>
-      <c r="Q156" s="4"/>
+      <c r="J156" s="3"/>
+      <c r="K156" s="3"/>
+      <c r="L156" s="3"/>
+      <c r="M156" s="3"/>
+      <c r="N156" s="3"/>
+      <c r="O156" s="3"/>
+      <c r="P156" s="3"/>
+      <c r="Q156" s="3"/>
       <c r="R156" s="3"/>
       <c r="S156" s="3"/>
       <c r="T156" s="3"/>
@@ -14295,14 +14298,14 @@
       <c r="G159" s="3"/>
       <c r="H159" s="3"/>
       <c r="I159" s="3"/>
-      <c r="J159" s="4"/>
-      <c r="K159" s="4"/>
-      <c r="L159" s="4"/>
-      <c r="M159" s="4"/>
-      <c r="N159" s="4"/>
-      <c r="O159" s="4"/>
-      <c r="P159" s="4"/>
-      <c r="Q159" s="4"/>
+      <c r="J159" s="3"/>
+      <c r="K159" s="3"/>
+      <c r="L159" s="3"/>
+      <c r="M159" s="3"/>
+      <c r="N159" s="3"/>
+      <c r="O159" s="3"/>
+      <c r="P159" s="3"/>
+      <c r="Q159" s="3"/>
       <c r="R159" s="3"/>
       <c r="S159" s="3"/>
       <c r="T159" s="3"/>
@@ -14343,14 +14346,14 @@
       <c r="G160" s="3"/>
       <c r="H160" s="3"/>
       <c r="I160" s="3"/>
-      <c r="J160" s="4"/>
-      <c r="K160" s="4"/>
-      <c r="L160" s="4"/>
-      <c r="M160" s="4"/>
-      <c r="N160" s="4"/>
-      <c r="O160" s="4"/>
-      <c r="P160" s="4"/>
-      <c r="Q160" s="4"/>
+      <c r="J160" s="3"/>
+      <c r="K160" s="3"/>
+      <c r="L160" s="3"/>
+      <c r="M160" s="3"/>
+      <c r="N160" s="3"/>
+      <c r="O160" s="3"/>
+      <c r="P160" s="3"/>
+      <c r="Q160" s="3"/>
       <c r="R160" s="3"/>
       <c r="S160" s="3"/>
       <c r="T160" s="3"/>
@@ -14465,14 +14468,14 @@
       <c r="G162" s="3"/>
       <c r="H162" s="3"/>
       <c r="I162" s="3"/>
-      <c r="J162" s="4"/>
-      <c r="K162" s="4"/>
-      <c r="L162" s="4"/>
-      <c r="M162" s="4"/>
-      <c r="N162" s="4"/>
-      <c r="O162" s="4"/>
-      <c r="P162" s="4"/>
-      <c r="Q162" s="4"/>
+      <c r="J162" s="3"/>
+      <c r="K162" s="3"/>
+      <c r="L162" s="3"/>
+      <c r="M162" s="3"/>
+      <c r="N162" s="3"/>
+      <c r="O162" s="3"/>
+      <c r="P162" s="3"/>
+      <c r="Q162" s="3"/>
       <c r="R162" s="3"/>
       <c r="S162" s="3"/>
       <c r="T162" s="3"/>
@@ -14513,14 +14516,14 @@
       <c r="G163" s="3"/>
       <c r="H163" s="3"/>
       <c r="I163" s="3"/>
-      <c r="J163" s="4"/>
-      <c r="K163" s="4"/>
-      <c r="L163" s="4"/>
-      <c r="M163" s="4"/>
-      <c r="N163" s="4"/>
-      <c r="O163" s="4"/>
-      <c r="P163" s="4"/>
-      <c r="Q163" s="4"/>
+      <c r="J163" s="3"/>
+      <c r="K163" s="3"/>
+      <c r="L163" s="3"/>
+      <c r="M163" s="3"/>
+      <c r="N163" s="3"/>
+      <c r="O163" s="3"/>
+      <c r="P163" s="3"/>
+      <c r="Q163" s="3"/>
       <c r="R163" s="3"/>
       <c r="S163" s="3"/>
       <c r="T163" s="3"/>
@@ -14561,14 +14564,14 @@
       <c r="G164" s="3"/>
       <c r="H164" s="3"/>
       <c r="I164" s="3"/>
-      <c r="J164" s="4"/>
-      <c r="K164" s="4"/>
-      <c r="L164" s="4"/>
-      <c r="M164" s="4"/>
-      <c r="N164" s="4"/>
-      <c r="O164" s="4"/>
-      <c r="P164" s="4"/>
-      <c r="Q164" s="4"/>
+      <c r="J164" s="3"/>
+      <c r="K164" s="3"/>
+      <c r="L164" s="3"/>
+      <c r="M164" s="3"/>
+      <c r="N164" s="3"/>
+      <c r="O164" s="3"/>
+      <c r="P164" s="3"/>
+      <c r="Q164" s="3"/>
       <c r="R164" s="3"/>
       <c r="S164" s="3"/>
       <c r="T164" s="3"/>
@@ -14609,14 +14612,14 @@
       <c r="G165" s="3"/>
       <c r="H165" s="3"/>
       <c r="I165" s="3"/>
-      <c r="J165" s="4"/>
-      <c r="K165" s="4"/>
-      <c r="L165" s="4"/>
-      <c r="M165" s="4"/>
-      <c r="N165" s="4"/>
-      <c r="O165" s="4"/>
-      <c r="P165" s="4"/>
-      <c r="Q165" s="4"/>
+      <c r="J165" s="3"/>
+      <c r="K165" s="3"/>
+      <c r="L165" s="3"/>
+      <c r="M165" s="3"/>
+      <c r="N165" s="3"/>
+      <c r="O165" s="3"/>
+      <c r="P165" s="3"/>
+      <c r="Q165" s="3"/>
       <c r="R165" s="3"/>
       <c r="S165" s="3"/>
       <c r="T165" s="3"/>

</xml_diff>